<commit_message>
Update card excel files
Signed-off-by: SkySakura <1693385825@qq.com>
</commit_message>
<xml_diff>
--- a/ExcelData/__enums__.xlsx
+++ b/ExcelData/__enums__.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace2\luban_examples\MiniTemplate\Datas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E1AAA0-A88D-4E41-AC05-256E9DB382D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>##var</t>
   </si>
@@ -77,13 +84,67 @@
   </si>
   <si>
     <t>注释</t>
+  </si>
+  <si>
+    <t>cardGame.EmotionType</t>
+  </si>
+  <si>
+    <t>Happy</t>
+  </si>
+  <si>
+    <t>喜悦</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t>悲伤</t>
+  </si>
+  <si>
+    <t>Angry</t>
+  </si>
+  <si>
+    <t>愤怒</t>
+  </si>
+  <si>
+    <t>cardGame.RareType</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>常见</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>稀有</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>史诗</t>
+  </si>
+  <si>
+    <t>SSR</t>
+  </si>
+  <si>
+    <t>限定</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +153,151 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,12 +306,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
+        <fgColor theme="9" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -135,9 +520,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -149,23 +776,67 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -423,32 +1094,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="5" width="14.125" customWidth="1"/>
-    <col min="6" max="6" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="20.8796296296296" customWidth="1"/>
+    <col min="4" max="5" width="14.1296296296296" customWidth="1"/>
+    <col min="6" max="6" width="9.37962962962963" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="5.25" customWidth="1"/>
-    <col min="10" max="10" width="12.125" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="10" max="10" width="12.1296296296296" customWidth="1"/>
+    <col min="11" max="11" width="15.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,15 +1141,15 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,14 +1175,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="99" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -534,12 +1205,107 @@
       </c>
       <c r="L3" s="1"/>
     </row>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="8:10">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="8:10">
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="8:10">
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="8:10">
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="8:10">
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:L1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>